<commit_message>
V1 - modified comment
</commit_message>
<xml_diff>
--- a/tokenizing-test-cases.xlsx
+++ b/tokenizing-test-cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DC\Desktop\Seneca\CPR101\CPR_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E030397A-09EF-47AE-BC04-DC5292074AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4797E1C-07C3-4FF7-83F0-CE5B1D2ABDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1185,8 +1185,55 @@
     <t>Sting input: Hello World! Today is 11 / 28 / 2023</t>
   </si>
   <si>
-    <t>Hello World! Today is 11 / 28 / 2023
-Word #1 is 'Hello'
+    <t xml:space="preserve"> + Normal case: test normal input with alphabets (both Upper and lower case), numbers and special characters. Separate with whitespace.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + Edge case: test the input with no string but the '\n' new line character</t>
+  </si>
+  <si>
+    <t>Prompt user to enter some words again</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + Normal case: quit the programming with character "q"</t>
+  </si>
+  <si>
+    <t>String input: q</t>
+  </si>
+  <si>
+    <t>The programming will leave the iteration and output a message of End of Demo</t>
+  </si>
+  <si>
+    <t>String input: Hello     World!(5 spaces)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + Edge case: test the input with mutiple withespace(delimiter) between words</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Normal case: test input start with a single 'q' followed by other words</t>
+  </si>
+  <si>
+    <t>String input: q Hello World!</t>
+  </si>
+  <si>
+    <t>The program should tokenize the words and go to next iteration to prompt user input some word again</t>
+  </si>
+  <si>
+    <t>The program print out the result of tokenized word and end with a ending message</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + Edge case: test the input with a whitespace(delimiter) only</t>
+  </si>
+  <si>
+    <t>String input: " "</t>
+  </si>
+  <si>
+    <t>no character, press keyboard 'enter' key only</t>
+  </si>
+  <si>
+    <t>Recommended fix: Logic should check if the string length is greater than 1 character. If the string length is greater than 1, then the iteration will continuous; if the string length is equal to 1 and the charater is 'q', then the iteration end.</t>
+  </si>
+  <si>
+    <t>Word #1 is 'Hello'
 Word #2 is 'World!'
 Word #3 is 'Today'
 Word #4 is 'is'
@@ -1197,57 +1244,8 @@
 Word #9 is '2023'</t>
   </si>
   <si>
-    <t xml:space="preserve"> + Normal case: test normal input with alphabets (both Upper and lower case), numbers and special characters. Separate with whitespace.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + Edge case: test the input with no string but the '\n' new line character</t>
-  </si>
-  <si>
-    <t>Prompt user to enter some words again</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + Normal case: quit the programming with character "q"</t>
-  </si>
-  <si>
-    <t>String input: q</t>
-  </si>
-  <si>
-    <t>The programming will leave the iteration and output a message of End of Demo</t>
-  </si>
-  <si>
-    <t>Hello     World!
-Word #1 is 'Hello'
+    <t>Word #1 is 'Hello'
 Word #2 is 'World!'</t>
-  </si>
-  <si>
-    <t>String input: Hello     World!(5 spaces)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + Edge case: test the input with mutiple withespace(delimiter) between words</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Normal case: test input start with a single 'q' followed by other words</t>
-  </si>
-  <si>
-    <t>String input: q Hello World!</t>
-  </si>
-  <si>
-    <t>The program should tokenize the words and go to next iteration to prompt user input some word again</t>
-  </si>
-  <si>
-    <t>The program print out the result of tokenized word and end with a ending message</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + Edge case: test the input with a whitespace(delimiter) only</t>
-  </si>
-  <si>
-    <t>String input: " "</t>
-  </si>
-  <si>
-    <t>no character, press keyboard 'enter' key only</t>
-  </si>
-  <si>
-    <t>Recommended fix: Logic should check if the string length is greater than 1 character. If the string length is greater than 1, then the iteration will continuous; if the string length is equal to 1 and the charater is 'q', then the iteration end.</t>
   </si>
 </sst>
 </file>
@@ -1791,6 +1789,33 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1802,33 +1827,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2188,22 +2186,22 @@
       <c r="B1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="41" t="str">
+      <c r="C1" s="50" t="str">
         <f>"Do not save or use this worksheet – sample test cases only"</f>
         <v>Do not save or use this worksheet – sample test cases only</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="27"/>
       <c r="F2" s="18" t="s">
         <v>11</v>
@@ -2315,7 +2313,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
@@ -2394,7 +2392,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2415,23 +2413,23 @@
       <c r="B1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="41" t="str">
+      <c r="C1" s="50" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As Tokenizing_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="2" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
       <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2440,19 +2438,19 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="41" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="21" t="s">
@@ -2462,64 +2460,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>42</v>
+      <c r="B4" s="44" t="s">
+        <v>41</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="46"/>
     </row>
     <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="50"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>55</v>
+      <c r="B6" s="44" t="s">
+        <v>53</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="50"/>
+      <c r="G6" s="46"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="48"/>
+      <c r="N6" s="44"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
     </row>
@@ -2527,75 +2525,75 @@
       <c r="A7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>50</v>
+      <c r="B7" s="44" t="s">
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="50"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="51"/>
+      <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="51" t="s">
-        <v>58</v>
+      <c r="G9" s="47" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="46" t="s">
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="G10" s="43" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2659,13 +2657,13 @@
       <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="20" t="s">
         <v>11</v>
       </c>

</xml_diff>